<commit_message>
Created methods that selects a random destination result item, selects the current day for check-in date and selects a checkout date within 2 weeks. Dynamic, randomized test case that can book a 2 week trip anywhere in the world
</commit_message>
<xml_diff>
--- a/com.bmwusa/src/test/resources/test_data.xlsx
+++ b/com.bmwusa/src/test/resources/test_data.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.bmwusa\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9B0764-F5DE-47FC-91F0-E3E757CA6369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43465CBF-DFAB-4178-A0E8-2CAE139AB29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{45A20FD9-8BD9-4FCD-8197-0CBE0A847F4A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
   <sheets>
-    <sheet name="bmwModels " sheetId="1" r:id="rId1"/>
+    <sheet name="nbaTeams" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="1" r:id="rId2"/>
+    <sheet name="bmwModels" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,63 +37,291 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+  <si>
+    <t>City Name</t>
+  </si>
+  <si>
+    <t>Team Name</t>
+  </si>
+  <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>Celtics</t>
+  </si>
+  <si>
+    <t>Brooklyn</t>
+  </si>
+  <si>
+    <t>Nets</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Cleveland</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>Detroit</t>
+  </si>
+  <si>
+    <t>Golden State</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Oklahoma City</t>
+  </si>
+  <si>
+    <t>Portland</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Milwaukee</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>Sacramento</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Orlando</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Memphis</t>
+  </si>
+  <si>
+    <t>New Orleans</t>
+  </si>
+  <si>
+    <t>San Antonio</t>
+  </si>
+  <si>
+    <t>Knicks</t>
+  </si>
+  <si>
+    <t>76ers</t>
+  </si>
+  <si>
+    <t>Raptors</t>
+  </si>
+  <si>
+    <t>Nuggets</t>
+  </si>
+  <si>
+    <t>Timberwolves</t>
+  </si>
+  <si>
+    <t>Thunder</t>
+  </si>
+  <si>
+    <t>Trail Blazers</t>
+  </si>
+  <si>
+    <t>Jazz</t>
+  </si>
+  <si>
+    <t>Bulls</t>
+  </si>
+  <si>
+    <t>Cavaliers</t>
+  </si>
+  <si>
+    <t>Pistons</t>
+  </si>
+  <si>
+    <t>Pacers</t>
+  </si>
+  <si>
+    <t>Bucks</t>
+  </si>
+  <si>
+    <t>Warriors</t>
+  </si>
+  <si>
+    <t>Clippers</t>
+  </si>
+  <si>
+    <t>Lakers</t>
+  </si>
+  <si>
+    <t>Suns</t>
+  </si>
+  <si>
+    <t>Kings</t>
+  </si>
+  <si>
+    <t>Hawks</t>
+  </si>
+  <si>
+    <t>Hornets</t>
+  </si>
+  <si>
+    <t>Heat</t>
+  </si>
+  <si>
+    <t>Magic</t>
+  </si>
+  <si>
+    <t>Wizards</t>
+  </si>
+  <si>
+    <t>Mavericks</t>
+  </si>
+  <si>
+    <t>Rockets</t>
+  </si>
+  <si>
+    <t>Grizzlies</t>
+  </si>
+  <si>
+    <t>Pelicans</t>
+  </si>
+  <si>
+    <t>Spurs</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Atlanta Hawks</t>
+  </si>
+  <si>
+    <t>Boston Celtics</t>
+  </si>
+  <si>
+    <t>Brooklyn Nets</t>
+  </si>
+  <si>
+    <t>Charlotte Hornets</t>
+  </si>
+  <si>
+    <t>Chicago Bulls</t>
+  </si>
+  <si>
+    <t>Cleveland Cavaliers</t>
+  </si>
+  <si>
+    <t>Dallas Mavericks</t>
+  </si>
+  <si>
+    <t>Detroit Pistons</t>
+  </si>
+  <si>
+    <t>Denver Nuggets</t>
+  </si>
+  <si>
+    <t>Golden State Warriors</t>
+  </si>
+  <si>
+    <t>Houston Rockets</t>
+  </si>
+  <si>
+    <t>Indiana Pacers</t>
+  </si>
+  <si>
+    <t>LA Clippers</t>
+  </si>
+  <si>
+    <t>Los Angeles Lakers</t>
+  </si>
+  <si>
+    <t>Memphis Grizzlies</t>
+  </si>
+  <si>
+    <t>Miami Heat</t>
+  </si>
+  <si>
+    <t>Milwaukee Bucks</t>
+  </si>
+  <si>
+    <t>Minnesota Timberwolves</t>
+  </si>
+  <si>
+    <t>New Orleans Pelicans</t>
+  </si>
+  <si>
+    <t>New York Knicks</t>
+  </si>
+  <si>
+    <t>Oklahoma City Thunder</t>
+  </si>
+  <si>
+    <t>Orlando Magic</t>
+  </si>
+  <si>
+    <t>Philadelphia 76ers</t>
+  </si>
+  <si>
+    <t>Phoenix Suns</t>
+  </si>
+  <si>
+    <t>Portland Trail Blazers</t>
+  </si>
+  <si>
+    <t>Sacramento Kings</t>
+  </si>
+  <si>
+    <t>San Antonio Spurs</t>
+  </si>
+  <si>
+    <t>Toronto Raptors</t>
+  </si>
+  <si>
+    <t>Utah Jazz</t>
+  </si>
+  <si>
+    <t>Washington Wizards</t>
+  </si>
+  <si>
+    <t>NBA Teams</t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
   <si>
     <t>X1</t>
-  </si>
-  <si>
-    <t>X2</t>
-  </si>
-  <si>
-    <t>X3</t>
-  </si>
-  <si>
-    <t>X4</t>
-  </si>
-  <si>
-    <t>X5</t>
-  </si>
-  <si>
-    <t>X6</t>
-  </si>
-  <si>
-    <t>X7</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>BMW Models</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>Z4</t>
-  </si>
-  <si>
-    <t>M Models</t>
-  </si>
-  <si>
-    <t>iX</t>
-  </si>
-  <si>
-    <t>i4</t>
-  </si>
-  <si>
-    <t>i7</t>
   </si>
 </sst>
 </file>
@@ -135,10 +365,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,116 +683,502 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16672743-BBCF-4F3F-B8A6-DE61B566DD51}">
-  <dimension ref="A1:A19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA23FD94-FD19-4660-99A3-376865924FBE}">
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.21875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="2" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65AF868F-1619-4058-BC1A-5F3E5C88CA24}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="16" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B31">
+    <sortCondition ref="A2:A31"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DBDB2A-BA3E-4DD2-85D1-84D270436187}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
trying to deal with 'Access Denied' message on Expedia
</commit_message>
<xml_diff>
--- a/com.bmwusa/src/test/resources/test_data.xlsx
+++ b/com.bmwusa/src/test/resources/test_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.bmwusa\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43465CBF-DFAB-4178-A0E8-2CAE139AB29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50AB4DD-393C-41A5-88B0-C6BA642A06B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
   <sheets>
     <sheet name="nbaTeams" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="1" r:id="rId2"/>
+    <sheet name="nbaCityNameTeamName" sheetId="1" r:id="rId2"/>
     <sheet name="bmwModels" sheetId="3" r:id="rId3"/>
+    <sheet name="myTrips" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="121">
   <si>
     <t>City Name</t>
   </si>
@@ -322,6 +323,84 @@
   </si>
   <si>
     <t>X1</t>
+  </si>
+  <si>
+    <t>Locations</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Istanbul</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Rome</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>X3</t>
+  </si>
+  <si>
+    <t>X4</t>
+  </si>
+  <si>
+    <t>X5</t>
+  </si>
+  <si>
+    <t>X6</t>
+  </si>
+  <si>
+    <t>X7</t>
+  </si>
+  <si>
+    <t>Z4</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>iX</t>
+  </si>
+  <si>
+    <t>i4</t>
+  </si>
+  <si>
+    <t>i7</t>
   </si>
 </sst>
 </file>
@@ -365,11 +444,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1160,22 +1243,207 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DBDB2A-BA3E-4DD2-85D1-84D270436187}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F428AD-AE09-447E-9CC1-5B40C17299F3}">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on method that will read from multiple columns (in progress)
</commit_message>
<xml_diff>
--- a/com.bmwusa/src/test/resources/test_data.xlsx
+++ b/com.bmwusa/src/test/resources/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.bmwusa\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50AB4DD-393C-41A5-88B0-C6BA642A06B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973CDB80-BF3B-4736-9B79-6B2137C466D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
   <sheets>
     <sheet name="nbaTeams" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="123">
   <si>
     <t>City Name</t>
   </si>
@@ -319,9 +319,6 @@
     <t>NBA Teams</t>
   </si>
   <si>
-    <t>Models</t>
-  </si>
-  <si>
     <t>X1</t>
   </si>
   <si>
@@ -401,6 +398,15 @@
   </si>
   <si>
     <t>i7</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>BMW</t>
   </si>
 </sst>
 </file>
@@ -1243,10 +1249,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DBDB2A-BA3E-4DD2-85D1-84D270436187}">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1254,99 +1260,105 @@
     <col min="1" max="1" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1359,7 +1371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F428AD-AE09-447E-9CC1-5B40C17299F3}">
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1368,7 +1380,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -1378,72 +1390,72 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added assertions to all bmw test cases
</commit_message>
<xml_diff>
--- a/com.bmwusa/src/test/resources/test_data.xlsx
+++ b/com.bmwusa/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.bmwusa\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973CDB80-BF3B-4736-9B79-6B2137C466D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F98020B-1AB8-41D0-87AF-3F2534E71E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="121">
   <si>
     <t>City Name</t>
   </si>
@@ -400,13 +400,7 @@
     <t>i7</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Model</t>
-  </si>
-  <si>
-    <t>BMW</t>
   </si>
 </sst>
 </file>
@@ -1252,7 +1246,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1264,15 +1258,10 @@
       <c r="A1" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>121</v>
-      </c>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B2" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pushing bank of america test cases
</commit_message>
<xml_diff>
--- a/com.bmwusa/src/test/resources/test_data.xlsx
+++ b/com.bmwusa/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.bmwusa\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED60B2DD-A62D-48E5-A076-38490F800C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7D3536-72A4-4C36-AB76-8C37EB34EC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="628" firstSheet="2" activeTab="2" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
@@ -631,9 +631,6 @@
     <t>netflix@live.com</t>
   </si>
   <si>
-    <t>Model</t>
-  </si>
-  <si>
     <t>X4</t>
   </si>
   <si>
@@ -659,6 +656,9 @@
   </si>
   <si>
     <t>i7</t>
+  </si>
+  <si>
+    <t>Models</t>
   </si>
 </sst>
 </file>
@@ -1911,14 +1911,14 @@
   <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A14"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -1938,22 +1938,22 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
@@ -1988,27 +1988,27 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
post class demo push
</commit_message>
<xml_diff>
--- a/com.bmwusa/src/test/resources/test_data.xlsx
+++ b/com.bmwusa/src/test/resources/test_data.xlsx
@@ -8,28 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.bmwusa\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FE7BF1-0958-4C95-8C6F-EF86A1478634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBABFF2-2F6F-461B-B357-B152ED540FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="628" firstSheet="2" activeTab="2" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="628" activeTab="2" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
   <sheets>
     <sheet name="nbaTeams" sheetId="2" r:id="rId1"/>
     <sheet name="nbaCityNameTeamName" sheetId="1" r:id="rId2"/>
     <sheet name="bmwModels" sheetId="3" r:id="rId3"/>
-    <sheet name="bmwBuildYourOwn" sheetId="17" r:id="rId4"/>
-    <sheet name="myTrips" sheetId="4" r:id="rId5"/>
-    <sheet name="usaCities" sheetId="5" r:id="rId6"/>
-    <sheet name="USMarket" sheetId="6" r:id="rId7"/>
-    <sheet name="EuropeMarket" sheetId="7" r:id="rId8"/>
-    <sheet name="AsiaMarket" sheetId="8" r:id="rId9"/>
-    <sheet name="FXMarket" sheetId="9" r:id="rId10"/>
-    <sheet name="SoFi" sheetId="10" r:id="rId11"/>
-    <sheet name="EndToEnd" sheetId="11" r:id="rId12"/>
-    <sheet name="Filters" sheetId="12" r:id="rId13"/>
-    <sheet name="SearchFunction" sheetId="13" r:id="rId14"/>
-    <sheet name="AddingToCart" sheetId="14" r:id="rId15"/>
-    <sheet name="EmailData" sheetId="15" r:id="rId16"/>
-    <sheet name="Sheet7" sheetId="16" r:id="rId17"/>
+    <sheet name="bmwBodyType" sheetId="18" r:id="rId4"/>
+    <sheet name="bmwBuildYourOwn" sheetId="17" r:id="rId5"/>
+    <sheet name="myTrips" sheetId="4" r:id="rId6"/>
+    <sheet name="usaCities" sheetId="5" r:id="rId7"/>
+    <sheet name="USMarket" sheetId="6" r:id="rId8"/>
+    <sheet name="EuropeMarket" sheetId="7" r:id="rId9"/>
+    <sheet name="AsiaMarket" sheetId="8" r:id="rId10"/>
+    <sheet name="FXMarket" sheetId="9" r:id="rId11"/>
+    <sheet name="SoFi" sheetId="10" r:id="rId12"/>
+    <sheet name="EndToEnd" sheetId="11" r:id="rId13"/>
+    <sheet name="Filters" sheetId="12" r:id="rId14"/>
+    <sheet name="SearchFunction" sheetId="13" r:id="rId15"/>
+    <sheet name="AddingToCart" sheetId="14" r:id="rId16"/>
+    <sheet name="EmailData" sheetId="15" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="211">
   <si>
     <t>City Name</t>
   </si>
@@ -681,6 +681,9 @@
   </si>
   <si>
     <t>BMW</t>
+  </si>
+  <si>
+    <t>Body Type</t>
   </si>
 </sst>
 </file>
@@ -1282,6 +1285,59 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49C24E1-9850-4CD1-93E4-6444FCFDA700}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CFA5A2A-8233-4E65-8C5F-7BB017E8CE28}">
   <dimension ref="A1:A7"/>
   <sheetViews>
@@ -1334,7 +1390,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{118B9C6B-8AE9-42E8-98F4-70336A109C11}">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -1371,7 +1427,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F62D41-B8EE-4DE6-9F5F-4482129EDE4A}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -1413,7 +1469,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C02C1B-51B7-4E69-85C9-D37BE79B3190}">
   <dimension ref="A1:A28"/>
   <sheetViews>
@@ -1569,7 +1625,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B50783AA-DBB6-4811-90F7-767ED9DFDE06}">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -1605,7 +1661,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{781051E6-4249-47E2-93C8-6F416AE6185C}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1631,7 +1687,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6879E9-8413-4450-BFB6-832F473E04EB}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1694,18 +1750,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C97AC20-6DC1-48C5-9925-A1CA85849984}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1983,10 +2027,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DBDB2A-BA3E-4DD2-85D1-84D270436187}">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2089,31 +2133,6 @@
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>209</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2121,6 +2140,53 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7AC1EA-6C05-4C2C-8826-6A66254612D9}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565460A0-8473-434F-9594-BF69B83F7141}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2148,7 +2214,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F428AD-AE09-447E-9CC1-5B40C17299F3}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -2247,7 +2313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F168171D-B480-4774-B7A1-6093E7D36237}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -2343,7 +2409,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8BD1A03-FB14-4B19-9037-B86FF547E44E}">
   <dimension ref="A1:A7"/>
   <sheetViews>
@@ -2395,7 +2461,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A997DFE-457D-4F60-A5E8-304110D14DE1}">
   <dimension ref="A1:A7"/>
   <sheetViews>
@@ -2444,57 +2510,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49C24E1-9850-4CD1-93E4-6444FCFDA700}">
-  <dimension ref="A1:A7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="23.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>